<commit_message>
updated gitignore path and updated sheet
</commit_message>
<xml_diff>
--- a/Rishik's Sheet.xlsx
+++ b/Rishik's Sheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RISHIK RAJ\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STUDY\Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D63563A3-87B1-4F04-AD36-2FC162F7919F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208F2EF1-DDE5-47DD-8CB0-F54F81D77F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="828" activeTab="1" xr2:uid="{3EA64179-E55C-4397-B9A7-37D947379E12}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
   <si>
     <t>Problem No</t>
   </si>
@@ -614,15 +614,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B4B32D-1834-4CE8-AC24-3A581F79EA55}">
   <dimension ref="A1:U456"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="N3" sqref="N3"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21" style="3" customWidth="1"/>
+    <col min="2" max="2" width="21" style="4" customWidth="1"/>
     <col min="3" max="3" width="19.6640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="10.88671875" style="4" customWidth="1"/>
     <col min="5" max="5" width="33" style="3" customWidth="1"/>
@@ -705,7 +705,7 @@
       <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="4" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="4"/>
@@ -747,7 +747,9 @@
       <c r="A3" s="4">
         <v>2</v>
       </c>
-      <c r="B3" s="8"/>
+      <c r="B3" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="C3" s="4"/>
       <c r="G3" s="6">
         <v>46034</v>
@@ -757,7 +759,9 @@
       <c r="A4" s="4">
         <v>3</v>
       </c>
-      <c r="B4" s="8"/>
+      <c r="B4" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="C4" s="4"/>
       <c r="G4" s="6">
         <v>46034</v>
@@ -767,7 +771,9 @@
       <c r="A5" s="4">
         <v>4</v>
       </c>
-      <c r="B5" s="8"/>
+      <c r="B5" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="G5" s="6">
         <v>46034</v>
@@ -777,7 +783,9 @@
       <c r="A6" s="4">
         <v>5</v>
       </c>
-      <c r="B6" s="8"/>
+      <c r="B6" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="C6" s="4"/>
       <c r="G6" s="6">
         <v>46034</v>
@@ -787,7 +795,9 @@
       <c r="A7" s="4">
         <v>6</v>
       </c>
-      <c r="B7" s="8"/>
+      <c r="B7" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="G7" s="6">
         <v>46035</v>
       </c>
@@ -796,7 +806,7 @@
       <c r="A8" s="4">
         <v>7</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="4" t="s">
         <v>16</v>
       </c>
       <c r="G8" s="6">
@@ -807,7 +817,9 @@
       <c r="A9" s="4">
         <v>8</v>
       </c>
-      <c r="B9" s="8"/>
+      <c r="B9" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="G9" s="6">
         <v>46035</v>
       </c>
@@ -816,7 +828,9 @@
       <c r="A10" s="4">
         <v>9</v>
       </c>
-      <c r="B10" s="8"/>
+      <c r="B10" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="G10" s="6">
         <v>46035</v>
       </c>
@@ -825,7 +839,9 @@
       <c r="A11" s="4">
         <v>10</v>
       </c>
-      <c r="B11" s="8"/>
+      <c r="B11" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="G11" s="6">
         <v>46035</v>
       </c>
@@ -834,7 +850,9 @@
       <c r="A12" s="4">
         <v>11</v>
       </c>
-      <c r="B12" s="8"/>
+      <c r="B12" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="G12" s="6">
         <v>46036</v>
       </c>
@@ -843,7 +861,9 @@
       <c r="A13" s="4">
         <v>12</v>
       </c>
-      <c r="B13" s="8"/>
+      <c r="B13" s="4" t="s">
+        <v>16</v>
+      </c>
       <c r="G13" s="6">
         <v>46036</v>
       </c>
@@ -852,7 +872,7 @@
       <c r="A14" s="4">
         <v>13</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="B14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="G14" s="6">
@@ -863,7 +883,9 @@
       <c r="A15" s="4">
         <v>14</v>
       </c>
-      <c r="B15" s="8"/>
+      <c r="B15" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="G15" s="6">
         <v>46036</v>
       </c>
@@ -1701,7 +1723,7 @@
       <c r="A145" s="4">
         <v>144</v>
       </c>
-      <c r="B145" s="3" t="s">
+      <c r="B145" s="4" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1709,7 +1731,7 @@
       <c r="A146" s="4">
         <v>145</v>
       </c>
-      <c r="B146" s="3" t="s">
+      <c r="B146" s="4" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1717,7 +1739,7 @@
       <c r="A147" s="4">
         <v>146</v>
       </c>
-      <c r="B147" s="3" t="s">
+      <c r="B147" s="4" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1725,7 +1747,7 @@
       <c r="A148" s="4">
         <v>147</v>
       </c>
-      <c r="B148" s="3" t="s">
+      <c r="B148" s="4" t="s">
         <v>34</v>
       </c>
     </row>
@@ -1733,7 +1755,7 @@
       <c r="A149" s="4">
         <v>148</v>
       </c>
-      <c r="B149" s="3" t="s">
+      <c r="B149" s="4" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1741,7 +1763,7 @@
       <c r="A150" s="4">
         <v>149</v>
       </c>
-      <c r="B150" s="3" t="s">
+      <c r="B150" s="4" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1749,7 +1771,7 @@
       <c r="A151" s="4">
         <v>150</v>
       </c>
-      <c r="B151" s="3" t="s">
+      <c r="B151" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1757,7 +1779,7 @@
       <c r="A152" s="4">
         <v>151</v>
       </c>
-      <c r="B152" s="3" t="s">
+      <c r="B152" s="4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1765,7 +1787,7 @@
       <c r="A153" s="4">
         <v>152</v>
       </c>
-      <c r="B153" s="3" t="s">
+      <c r="B153" s="4" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1773,7 +1795,7 @@
       <c r="A154" s="4">
         <v>153</v>
       </c>
-      <c r="B154" s="3" t="s">
+      <c r="B154" s="4" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1781,7 +1803,7 @@
       <c r="A155" s="4">
         <v>154</v>
       </c>
-      <c r="B155" s="3" t="s">
+      <c r="B155" s="4" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1789,7 +1811,7 @@
       <c r="A156" s="4">
         <v>155</v>
       </c>
-      <c r="B156" s="3" t="s">
+      <c r="B156" s="4" t="s">
         <v>30</v>
       </c>
     </row>
@@ -3295,13 +3317,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:R1" xr:uid="{A1B4B32D-1834-4CE8-AC24-3A581F79EA55}"/>
-  <mergeCells count="7">
+  <mergeCells count="4">
     <mergeCell ref="B64:B96"/>
     <mergeCell ref="B97:B112"/>
     <mergeCell ref="B113:B144"/>
-    <mergeCell ref="B2:B7"/>
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="B14:B15"/>
     <mergeCell ref="B23:B63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added backend filter control
</commit_message>
<xml_diff>
--- a/Rishik's Sheet.xlsx
+++ b/Rishik's Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STUDY\Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{208F2EF1-DDE5-47DD-8CB0-F54F81D77F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1ADCE2-CF22-48F3-9623-B5BD002014BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="828" activeTab="1" xr2:uid="{3EA64179-E55C-4397-B9A7-37D947379E12}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
   <si>
     <t>Problem No</t>
   </si>
@@ -615,8 +615,8 @@
   <dimension ref="A1:U456"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -971,7 +971,7 @@
       <c r="A23" s="4">
         <v>22</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="B23" s="4" t="s">
         <v>26</v>
       </c>
       <c r="G23" s="6">
@@ -982,7 +982,9 @@
       <c r="A24" s="4">
         <v>23</v>
       </c>
-      <c r="B24" s="8"/>
+      <c r="B24" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="G24" s="6">
         <v>46038</v>
       </c>
@@ -991,7 +993,9 @@
       <c r="A25" s="4">
         <v>24</v>
       </c>
-      <c r="B25" s="8"/>
+      <c r="B25" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="G25" s="6">
         <v>46038</v>
       </c>
@@ -1000,7 +1004,9 @@
       <c r="A26" s="4">
         <v>25</v>
       </c>
-      <c r="B26" s="8"/>
+      <c r="B26" s="4" t="s">
+        <v>26</v>
+      </c>
       <c r="G26" s="6">
         <v>46038</v>
       </c>
@@ -1009,223 +1015,297 @@
       <c r="A27" s="4">
         <v>26</v>
       </c>
-      <c r="B27" s="8"/>
+      <c r="B27" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>27</v>
       </c>
-      <c r="B28" s="8"/>
+      <c r="B28" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="4">
         <v>28</v>
       </c>
-      <c r="B29" s="8"/>
+      <c r="B29" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>29</v>
       </c>
-      <c r="B30" s="8"/>
+      <c r="B30" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>30</v>
       </c>
-      <c r="B31" s="8"/>
+      <c r="B31" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="8"/>
+      <c r="B32" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>32</v>
       </c>
-      <c r="B33" s="8"/>
+      <c r="B33" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>33</v>
       </c>
-      <c r="B34" s="8"/>
+      <c r="B34" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" s="4">
         <v>34</v>
       </c>
-      <c r="B35" s="8"/>
+      <c r="B35" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>35</v>
       </c>
-      <c r="B36" s="8"/>
+      <c r="B36" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="8"/>
+      <c r="B37" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>37</v>
       </c>
-      <c r="B38" s="8"/>
+      <c r="B38" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>38</v>
       </c>
-      <c r="B39" s="8"/>
+      <c r="B39" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>39</v>
       </c>
-      <c r="B40" s="8"/>
+      <c r="B40" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>40</v>
       </c>
-      <c r="B41" s="8"/>
+      <c r="B41" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="4">
         <v>41</v>
       </c>
-      <c r="B42" s="8"/>
+      <c r="B42" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>42</v>
       </c>
-      <c r="B43" s="8"/>
+      <c r="B43" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>43</v>
       </c>
-      <c r="B44" s="8"/>
+      <c r="B44" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>44</v>
       </c>
-      <c r="B45" s="8"/>
+      <c r="B45" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" s="4">
         <v>45</v>
       </c>
-      <c r="B46" s="8"/>
+      <c r="B46" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>46</v>
       </c>
-      <c r="B47" s="8"/>
+      <c r="B47" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>47</v>
       </c>
-      <c r="B48" s="8"/>
+      <c r="B48" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" s="4">
         <v>48</v>
       </c>
-      <c r="B49" s="8"/>
+      <c r="B49" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>49</v>
       </c>
-      <c r="B50" s="8"/>
+      <c r="B50" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>50</v>
       </c>
-      <c r="B51" s="8"/>
+      <c r="B51" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" s="4">
         <v>51</v>
       </c>
-      <c r="B52" s="8"/>
+      <c r="B52" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>52</v>
       </c>
-      <c r="B53" s="8"/>
+      <c r="B53" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>53</v>
       </c>
-      <c r="B54" s="8"/>
+      <c r="B54" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" s="4">
         <v>54</v>
       </c>
-      <c r="B55" s="8"/>
+      <c r="B55" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" s="4">
         <v>55</v>
       </c>
-      <c r="B56" s="8"/>
+      <c r="B56" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" s="4">
         <v>56</v>
       </c>
-      <c r="B57" s="8"/>
+      <c r="B57" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>57</v>
       </c>
-      <c r="B58" s="8"/>
+      <c r="B58" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" s="4">
         <v>58</v>
       </c>
-      <c r="B59" s="8"/>
+      <c r="B59" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>59</v>
       </c>
-      <c r="B60" s="8"/>
+      <c r="B60" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" s="4">
         <v>60</v>
       </c>
-      <c r="B61" s="8"/>
+      <c r="B61" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" s="4">
         <v>61</v>
       </c>
-      <c r="B62" s="8"/>
+      <c r="B62" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
         <v>62</v>
       </c>
-      <c r="B63" s="8"/>
+      <c r="B63" s="4" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" s="4">
@@ -3317,11 +3397,10 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:R1" xr:uid="{A1B4B32D-1834-4CE8-AC24-3A581F79EA55}"/>
-  <mergeCells count="4">
+  <mergeCells count="3">
     <mergeCell ref="B64:B96"/>
     <mergeCell ref="B97:B112"/>
     <mergeCell ref="B113:B144"/>
-    <mergeCell ref="B23:B63"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added concept row in excel
</commit_message>
<xml_diff>
--- a/Rishik's Sheet.xlsx
+++ b/Rishik's Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\STUDY\Interview\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD1ADCE2-CF22-48F3-9623-B5BD002014BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E9E6B9-B7ED-4ABF-BD72-30DEFFF0D541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="828" activeTab="1" xr2:uid="{3EA64179-E55C-4397-B9A7-37D947379E12}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="828" activeTab="3" xr2:uid="{3EA64179-E55C-4397-B9A7-37D947379E12}"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="53">
   <si>
     <t>Problem No</t>
   </si>
@@ -189,6 +189,12 @@
   </si>
   <si>
     <t>Next Solve Date 2</t>
+  </si>
+  <si>
+    <t>2 pointer</t>
+  </si>
+  <si>
+    <t>Bit</t>
   </si>
 </sst>
 </file>
@@ -614,9 +620,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1B4B32D-1834-4CE8-AC24-3A581F79EA55}">
   <dimension ref="A1:U456"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C159" sqref="C159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1799,7 +1805,7 @@
       </c>
       <c r="B144" s="8"/>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" s="4">
         <v>144</v>
       </c>
@@ -1807,7 +1813,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" s="4">
         <v>145</v>
       </c>
@@ -1815,7 +1821,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" s="4">
         <v>146</v>
       </c>
@@ -1823,7 +1829,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A148" s="4">
         <v>147</v>
       </c>
@@ -1831,7 +1837,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="4">
         <v>148</v>
       </c>
@@ -1839,7 +1845,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" s="4">
         <v>149</v>
       </c>
@@ -1847,7 +1853,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" s="4">
         <v>150</v>
       </c>
@@ -1855,7 +1861,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" s="4">
         <v>151</v>
       </c>
@@ -1863,7 +1869,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" s="4">
         <v>152</v>
       </c>
@@ -1871,7 +1877,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" s="4">
         <v>153</v>
       </c>
@@ -1879,7 +1885,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" s="4">
         <v>154</v>
       </c>
@@ -1887,7 +1893,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" s="4">
         <v>155</v>
       </c>
@@ -1895,22 +1901,34 @@
         <v>30</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" s="4">
         <v>156</v>
       </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B157" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" s="4">
         <v>157</v>
       </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B158" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" s="4">
         <v>158</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" s="4">
         <v>159</v>
       </c>
@@ -3422,7 +3440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446591B3-AE61-4BA9-BA39-D212CC14DDC6}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>

</xml_diff>